<commit_message>
extra cred lab in progress
</commit_message>
<xml_diff>
--- a/lab11/spreadsheet.xlsx
+++ b/lab11/spreadsheet.xlsx
@@ -250,7 +250,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -812,12 +812,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="31974352"/>
-        <c:axId val="95642927"/>
-        <c:axId val="73213786"/>
+        <c:axId val="12875631"/>
+        <c:axId val="1920953"/>
+        <c:axId val="2498574"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="31974352"/>
+        <c:axId val="12875631"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -873,7 +873,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95642927"/>
+        <c:crossAx val="1920953"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -881,7 +881,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95642927"/>
+        <c:axId val="1920953"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -947,12 +947,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31974352"/>
+        <c:crossAx val="12875631"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="73213786"/>
+        <c:axId val="2498574"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1008,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95642927"/>
+        <c:crossAx val="1920953"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1047,7 +1047,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1423,11 +1423,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="2979935"/>
-        <c:axId val="88473147"/>
+        <c:axId val="61538249"/>
+        <c:axId val="29075016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2979935"/>
+        <c:axId val="61538249"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1483,7 +1483,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88473147"/>
+        <c:crossAx val="29075016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1491,7 +1491,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88473147"/>
+        <c:axId val="29075016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1556,7 +1556,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2979935"/>
+        <c:crossAx val="61538249"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1604,7 +1604,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2106,12 +2106,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="box"/>
-        <c:axId val="88614588"/>
-        <c:axId val="49132405"/>
-        <c:axId val="74300583"/>
+        <c:axId val="34466510"/>
+        <c:axId val="82754610"/>
+        <c:axId val="35228085"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="88614588"/>
+        <c:axId val="34466510"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2167,7 +2167,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49132405"/>
+        <c:crossAx val="82754610"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2175,7 +2175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49132405"/>
+        <c:axId val="82754610"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2240,12 +2240,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88614588"/>
+        <c:crossAx val="34466510"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="74300583"/>
+        <c:axId val="35228085"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2301,7 +2301,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49132405"/>
+        <c:crossAx val="82754610"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -3105,8 +3105,8 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A85" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C116" activeCellId="0" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>